<commit_message>
Second draft update, along with the necessary tables and figures. Updated SCM results. Still need to do the supporting information.
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaCaCl2Oxic/RaCaCl2Oxic Equilibrated Data.xlsx
+++ b/Sorption Experiments/RaCaCl2Oxic/RaCaCl2Oxic Equilibrated Data.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Sorption Experiments\RaCaCl2Oxic\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Equilibrated Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -72,8 +67,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,14 +131,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -190,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,10 +209,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,7 +243,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,19 +418,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,158 +433,158 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>20.53</v>
+        <v>20.30291666666667</v>
       </c>
       <c r="C2">
-        <v>0.36954000000000009</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3677365781250001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>20.627500000000001</v>
+        <v>20.27395833333333</v>
       </c>
       <c r="C3">
-        <v>0.37129499999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.36797234375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>19.085000000000001</v>
+        <v>19.29708333333333</v>
       </c>
       <c r="C4">
-        <v>0.35688950000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.35892575</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>19.821666666666669</v>
+        <v>19.72104166666666</v>
       </c>
       <c r="C5">
-        <v>0.36273650000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.362374140625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>19.85166666666667</v>
+        <v>20.00041666666667</v>
       </c>
       <c r="C6">
-        <v>0.36328549999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.365257609375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>15.37333333333333</v>
+        <v>15.34416666666667</v>
       </c>
       <c r="C7">
-        <v>0.32053399999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.319925875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>16.326666666666672</v>
+        <v>15.99166666666667</v>
       </c>
       <c r="C8">
-        <v>0.32979866666666668</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3264298958333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>15.660833333333329</v>
+        <v>15.614375</v>
       </c>
       <c r="C9">
-        <v>0.32339620833333338</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.322827203125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>13.317500000000001</v>
+        <v>13.18</v>
       </c>
       <c r="C10">
-        <v>0.29831200000000008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.29671475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>13.069166666666669</v>
+        <v>12.936875</v>
       </c>
       <c r="C11">
-        <v>0.29470970833333332</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2935053515625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>13.68</v>
+        <v>13.50416666666667</v>
       </c>
       <c r="C12">
-        <v>0.30232799999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2999613020833333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>18.002500000000001</v>
+        <v>17.84479166666667</v>
       </c>
       <c r="C13">
-        <v>0.34654812499999987</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.34529671875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>18.181666666666668</v>
+        <v>17.93</v>
       </c>
       <c r="C14">
-        <v>0.34817891666666673</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.34560075</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>17.391666666666669</v>
+        <v>17.56416666666667</v>
       </c>
       <c r="C15">
-        <v>0.34000708333333329</v>
+        <v>0.3422816979166666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>